<commit_message>
PBStools 1.43.8 (2025-04-23)  [Rcheck=T, Rbuild=T]   * Rcode     + Modified function `calcMA' to deal with moving-average window more accurately (RH 250416)     + Added function `smoothPDO' to smooth environmental anomalies (RH 250416)     + Updated functions `adjustMajor', `getData', and `linguaFranca' (RH 230423)   * Scode     + Updated `gfb_bio.sql' to account for the combination areas created by the new shoreside biosampling program (RH 250423)   * Documentation     + Added french version of the catch reconstruction pdf (RH 250423)
</commit_message>
<xml_diff>
--- a/PBStools/inst/sql/bio.fields.xlsx
+++ b/PBStools/inst/sql/bio.fields.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="7740" firstSheet="11" activeTab="18"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="7740" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="bio.fields" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9186" uniqueCount="6534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9236" uniqueCount="6582">
   <si>
     <t>EID</t>
   </si>
@@ -19648,13 +19648,157 @@
   </si>
   <si>
     <t>Jig surveys</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>3CD: WEST COAST VANCOUVER ISLAND</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>3D5A: N.W. VANCOUVER ISLAND AND SOUTHERN Q.C. SOUND</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>5AB: QUEEN CHARLOTTE SOUND</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>5BC: NORTHERN Q.C. SOUND AND SOUTHERN HECATE STRAIT</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>5CD: HECATE STRAIT</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>5DE: NORTHERN HECATE STRAIT AND WEST COAST HAIDA GWAII</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>5BE: NORTHERN Q.C. SOUND AND WEST COAST HAIDA GWAII</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>3CD</t>
+  </si>
+  <si>
+    <t>5AB</t>
+  </si>
+  <si>
+    <t>5BC</t>
+  </si>
+  <si>
+    <t>5CD</t>
+  </si>
+  <si>
+    <t>5DE</t>
+  </si>
+  <si>
+    <t>5BE</t>
+  </si>
+  <si>
+    <t>3D5A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -19825,6 +19969,16 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="36">
@@ -20185,7 +20339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -20234,8 +20388,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -20317,8 +20472,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="12" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -20358,6 +20519,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_ameth" xfId="42"/>
     <cellStyle name="Normal_ART" xfId="44"/>
+    <cellStyle name="Normal_major" xfId="48"/>
     <cellStyle name="Normal_mat.conv" xfId="45"/>
     <cellStyle name="Normal_mat.rf" xfId="46"/>
     <cellStyle name="Normal_source" xfId="47"/>
@@ -43105,10 +43267,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -43117,297 +43279,385 @@
     <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="35" t="s">
         <v>332</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="35" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="36" t="s">
+        <v>6534</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>334</v>
       </c>
       <c r="C2" t="s">
         <v>1076</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="36" t="s">
+        <v>6535</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="36" t="s">
+        <v>6536</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>335</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="36" t="s">
+        <v>6537</v>
+      </c>
+      <c r="B5" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="36" t="s">
+        <v>6538</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>337</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="36" t="s">
+        <v>6539</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>338</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="36" t="s">
+        <v>6540</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>339</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="36" t="s">
+        <v>6541</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="36" t="s">
+        <v>6542</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>341</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="36" t="s">
+        <v>6543</v>
+      </c>
+      <c r="B11" s="36" t="s">
         <v>342</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="36" t="s">
+        <v>6544</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>1055</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="36" t="s">
+        <v>6545</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="36" t="s">
+        <v>6546</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>345</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" s="36" t="s">
+        <v>6547</v>
+      </c>
+      <c r="B15" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>1063</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="36" t="s">
+        <v>6548</v>
+      </c>
+      <c r="B16" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="36" t="s">
+        <v>6549</v>
+      </c>
+      <c r="B17" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:3" ht="15">
+      <c r="A18" s="36" t="s">
+        <v>6550</v>
+      </c>
+      <c r="B18" s="36" t="s">
         <v>349</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>1066</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:3" ht="15">
+      <c r="A19" s="36" t="s">
+        <v>6551</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>350</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>61</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="36" t="s">
+        <v>6552</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>351</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>1068</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:3" ht="15">
+      <c r="A21" s="36" t="s">
+        <v>6553</v>
+      </c>
+      <c r="B21" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>1069</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>63</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="36" t="s">
+        <v>6554</v>
+      </c>
+      <c r="B22" s="36" t="s">
         <v>353</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>1070</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:3" ht="15">
+      <c r="A23" s="36" t="s">
+        <v>6555</v>
+      </c>
+      <c r="B23" s="36" t="s">
         <v>354</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>1071</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>65</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:3" ht="15">
+      <c r="A24" s="36" t="s">
+        <v>6556</v>
+      </c>
+      <c r="B24" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>1072</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:3" ht="15">
+      <c r="A25" s="36" t="s">
+        <v>6557</v>
+      </c>
+      <c r="B25" s="36" t="s">
         <v>356</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>67</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:3" ht="15">
+      <c r="A26" s="36" t="s">
+        <v>6558</v>
+      </c>
+      <c r="B26" s="36" t="s">
         <v>357</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>1074</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>68</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" s="36" t="s">
+        <v>6559</v>
+      </c>
+      <c r="B27" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>1075</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>99</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" s="36" t="s">
+        <v>6560</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>6561</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6575</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15">
+      <c r="A29" s="36" t="s">
+        <v>6562</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>6563</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6581</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15">
+      <c r="A30" s="36" t="s">
+        <v>6564</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>6565</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6576</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15">
+      <c r="A31" s="36" t="s">
+        <v>6566</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>6567</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6577</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="36" t="s">
+        <v>6568</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>6569</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6578</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="36" t="s">
+        <v>6570</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>6571</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6579</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15">
+      <c r="A34" s="36" t="s">
+        <v>6572</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>6573</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6580</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15">
+      <c r="A35" s="36" t="s">
+        <v>6574</v>
+      </c>
+      <c r="B35" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C35" t="s">
         <v>1076</v>
       </c>
     </row>
@@ -52421,7 +52671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection sqref="A1:B86"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PBStools 1.43.9 (2025-06-09)  [Rcheck=T, Rbuild=T]   * R code     + Added revised code for the function `buildCatch' [M07] (RH 250526)     + Fixed small bug in function `getData' [M01] (RH 250528)     + Modified function `compAF' [M06] to better handle the labelling of binned-year panels (RH 250604)     + Modified function `linguaFranca' [M01] (RH 250604)     + Added e-grave to menu in function `convUTF' [M01] (RH 250604)     + Revised function `adjustMajor' [M01] to deal with combo-majors in GFBioSQL from the new shoreside BSP (RH 250605)     + Tweaked colours in function `weightBio' [M02] (RH 250605)
</commit_message>
<xml_diff>
--- a/PBStools/inst/sql/bio.fields.xlsx
+++ b/PBStools/inst/sql/bio.fields.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="7740" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="7740" firstSheet="11" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="bio.fields" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9236" uniqueCount="6582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9269" uniqueCount="6610">
   <si>
     <t>EID</t>
   </si>
@@ -19792,13 +19792,97 @@
   </si>
   <si>
     <t>3D5A</t>
+  </si>
+  <si>
+    <t>FISHERY_SECTOR</t>
+  </si>
+  <si>
+    <t>NSECTOR</t>
+  </si>
+  <si>
+    <t>FOREIGN</t>
+  </si>
+  <si>
+    <t>GROUNDFISH LONGLINE</t>
+  </si>
+  <si>
+    <t>GROUNDFISH TRAWL</t>
+  </si>
+  <si>
+    <t>HALIBUT</t>
+  </si>
+  <si>
+    <t>HALIBUT AND SABLEFISH</t>
+  </si>
+  <si>
+    <t>K/L</t>
+  </si>
+  <si>
+    <t>K/ZN</t>
+  </si>
+  <si>
+    <t>ROCKFISH INSIDE</t>
+  </si>
+  <si>
+    <t>ROCKFISH OUTSIDE</t>
+  </si>
+  <si>
+    <t>SCHEDULE II</t>
+  </si>
+  <si>
+    <t>SPINY DOGFISH</t>
+  </si>
+  <si>
+    <t>ZN</t>
+  </si>
+  <si>
+    <t>GFFOS FISHERY_SECTOR</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>acro</t>
+  </si>
+  <si>
+    <t>GFT</t>
+  </si>
+  <si>
+    <t>KZN</t>
+  </si>
+  <si>
+    <t>LIN</t>
+  </si>
+  <si>
+    <t>RFO</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>FOR</t>
+  </si>
+  <si>
+    <t>ZNR</t>
+  </si>
+  <si>
+    <t>HAS</t>
+  </si>
+  <si>
+    <t>KOL</t>
+  </si>
+  <si>
+    <t>GLL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -19974,11 +20058,23 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="36">
@@ -20339,7 +20435,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -20389,8 +20485,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -20478,8 +20575,15 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="12" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -20519,6 +20623,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_ameth" xfId="42"/>
     <cellStyle name="Normal_ART" xfId="44"/>
+    <cellStyle name="Normal_fid" xfId="49"/>
     <cellStyle name="Normal_major" xfId="48"/>
     <cellStyle name="Normal_mat.conv" xfId="45"/>
     <cellStyle name="Normal_mat.rf" xfId="46"/>
@@ -43269,7 +43374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28:C34"/>
     </sheetView>
   </sheetViews>
@@ -67176,18 +67281,19 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" activeCellId="1" sqref="A14:A27 D14:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1030</v>
       </c>
@@ -67198,7 +67304,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -67209,7 +67315,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -67220,7 +67326,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -67231,7 +67337,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -67242,7 +67348,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -67253,7 +67359,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>8</v>
       </c>
@@ -67264,7 +67370,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>9</v>
       </c>
@@ -67275,7 +67381,225 @@
         <v>1045</v>
       </c>
     </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>6596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="A13" s="37" t="s">
+        <v>6582</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>6583</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6597</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" s="38" t="s">
+        <v>6584</v>
+      </c>
+      <c r="B14" s="39">
+        <v>33040</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15">
+      <c r="A15" s="38" t="s">
+        <v>6585</v>
+      </c>
+      <c r="B15" s="39">
+        <v>8900</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" s="38" t="s">
+        <v>6586</v>
+      </c>
+      <c r="B16" s="39">
+        <v>5671167</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15">
+      <c r="A17" s="38" t="s">
+        <v>6587</v>
+      </c>
+      <c r="B17" s="39">
+        <v>1009333</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15">
+      <c r="A18" s="38" t="s">
+        <v>6588</v>
+      </c>
+      <c r="B18" s="39">
+        <v>423797</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15">
+      <c r="A19" s="38" t="s">
+        <v>6589</v>
+      </c>
+      <c r="B19" s="39">
+        <v>1137</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15">
+      <c r="A20" s="38" t="s">
+        <v>6590</v>
+      </c>
+      <c r="B20" s="39">
+        <v>66</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15">
+      <c r="A21" s="38" t="s">
+        <v>6349</v>
+      </c>
+      <c r="B21" s="39">
+        <v>85577</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6601</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15">
+      <c r="A22" s="38" t="s">
+        <v>6591</v>
+      </c>
+      <c r="B22" s="39">
+        <v>50723</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6602</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15">
+      <c r="A23" s="38" t="s">
+        <v>6592</v>
+      </c>
+      <c r="B23" s="39">
+        <v>306628</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6603</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15">
+      <c r="A24" s="38" t="s">
+        <v>6344</v>
+      </c>
+      <c r="B24" s="39">
+        <v>361188</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15">
+      <c r="A25" s="38" t="s">
+        <v>6593</v>
+      </c>
+      <c r="B25" s="39">
+        <v>73408</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15">
+      <c r="A26" s="38" t="s">
+        <v>6594</v>
+      </c>
+      <c r="B26" s="39">
+        <v>68494</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15">
+      <c r="A27" s="38" t="s">
+        <v>6595</v>
+      </c>
+      <c r="B27" s="39">
+        <v>622193</v>
+      </c>
+      <c r="C27">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6606</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A14:B27">
+    <sortCondition ref="A14:A27"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>